<commit_message>
quickfix: stack pointer as source encoding
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev 4).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev 4).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:E79"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4643,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,10 +5094,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C26" s="44">
         <v>3</v>
@@ -5105,10 +5105,10 @@
       <c r="D26" s="52" t="s">
         <v>335</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="41" t="s">
         <v>286</v>
       </c>
       <c r="G26" s="18"/>
@@ -5199,25 +5199,25 @@
       <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="46"/>
       <c r="D33" s="53"/>
       <c r="E33" s="24" t="s">
         <v>231</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>349</v>
-      </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="29"/>
+        <v>288</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C34" s="44">
         <v>3</v>
@@ -5225,10 +5225,10 @@
       <c r="D34" s="52" t="s">
         <v>335</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F34" s="41" t="s">
+      <c r="F34" s="42" t="s">
         <v>286</v>
       </c>
       <c r="G34" s="18"/>
@@ -5319,18 +5319,18 @@
       <c r="H40" s="29"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="46"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="53"/>
       <c r="E41" s="24" t="s">
         <v>231</v>
       </c>
       <c r="F41" s="43" t="s">
-        <v>288</v>
-      </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="27"/>
+        <v>349</v>
+      </c>
+      <c r="G41" s="20"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">

</xml_diff>